<commit_message>
K_NN modificado e imagenes añadidas.
</commit_message>
<xml_diff>
--- a/nearest_neightbours.xlsx
+++ b/nearest_neightbours.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +482,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -491,13 +491,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -511,25 +511,25 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -540,28 +540,28 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>12</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11</v>
+      </c>
+      <c r="F4" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
-        <v>16</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -569,25 +569,25 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -598,28 +598,28 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" t="n">
         <v>12</v>
       </c>
-      <c r="E6" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" t="n">
-        <v>11</v>
-      </c>
       <c r="G6" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -627,28 +627,28 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G7" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H7" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -656,28 +656,28 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="G8" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H8" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -694,19 +694,19 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E9" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -734,16 +734,16 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G11" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -766,16 +766,16 @@
         <v>11</v>
       </c>
       <c r="E12" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G12" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -792,19 +792,19 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G13" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H13" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -812,28 +812,28 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" t="n">
         <v>15</v>
       </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
       <c r="G14" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H14" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -841,28 +841,28 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G15" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -870,28 +870,28 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F16" t="n">
+        <v>13</v>
+      </c>
+      <c r="G16" t="n">
+        <v>6</v>
+      </c>
+      <c r="H16" t="n">
         <v>1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" t="n">
-        <v>12</v>
-      </c>
-      <c r="H16" t="n">
-        <v>5</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -908,19 +908,19 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G17" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -937,16 +937,16 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F18" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -977,16 +977,16 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G20" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -1006,16 +1006,16 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E21" t="n">
         <v>13</v>
       </c>
       <c r="F21" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G21" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -1035,19 +1035,19 @@
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G22" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -1055,28 +1055,28 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G23" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H23" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1084,28 +1084,28 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G24" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -1113,28 +1113,28 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G25" t="n">
         <v>15</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
@@ -1151,19 +1151,19 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B27" t="n">
         <v>0</v>
@@ -1183,16 +1183,16 @@
         <v>2</v>
       </c>
       <c r="E27" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G27" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
@@ -1209,6 +1209,492 @@
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
     </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5</v>
+      </c>
+      <c r="F29" t="n">
+        <v>14</v>
+      </c>
+      <c r="G29" t="n">
+        <v>12</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>7</v>
+      </c>
+      <c r="E30" t="n">
+        <v>15</v>
+      </c>
+      <c r="F30" t="n">
+        <v>8</v>
+      </c>
+      <c r="G30" t="n">
+        <v>14</v>
+      </c>
+      <c r="H30" t="n">
+        <v>4</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>6</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" t="n">
+        <v>13</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>13</v>
+      </c>
+      <c r="G32" t="n">
+        <v>4</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>3</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>11</v>
+      </c>
+      <c r="F33" t="n">
+        <v>9</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8</v>
+      </c>
+      <c r="D34" t="n">
+        <v>16</v>
+      </c>
+      <c r="E34" t="n">
+        <v>13</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>3</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>5</v>
+      </c>
+      <c r="D35" t="n">
+        <v>14</v>
+      </c>
+      <c r="E35" t="n">
+        <v>16</v>
+      </c>
+      <c r="F35" t="n">
+        <v>11</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>6</v>
+      </c>
+      <c r="F36" t="n">
+        <v>12</v>
+      </c>
+      <c r="G36" t="n">
+        <v>13</v>
+      </c>
+      <c r="H36" t="n">
+        <v>3</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>3</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6</v>
+      </c>
+      <c r="F38" t="n">
+        <v>15</v>
+      </c>
+      <c r="G38" t="n">
+        <v>6</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>3</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>11</v>
+      </c>
+      <c r="E39" t="n">
+        <v>13</v>
+      </c>
+      <c r="F39" t="n">
+        <v>8</v>
+      </c>
+      <c r="G39" t="n">
+        <v>11</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>3</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>9</v>
+      </c>
+      <c r="D40" t="n">
+        <v>13</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>9</v>
+      </c>
+      <c r="G40" t="n">
+        <v>10</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>3</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>8</v>
+      </c>
+      <c r="D41" t="n">
+        <v>9</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3</v>
+      </c>
+      <c r="F41" t="n">
+        <v>15</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>3</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>5</v>
+      </c>
+      <c r="F42" t="n">
+        <v>14</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>3</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>3</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>5</v>
+      </c>
+      <c r="G43" t="n">
+        <v>13</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>3</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>9</v>
+      </c>
+      <c r="E44" t="n">
+        <v>12</v>
+      </c>
+      <c r="F44" t="n">
+        <v>5</v>
+      </c>
+      <c r="G44" t="n">
+        <v>10</v>
+      </c>
+      <c r="H44" t="n">
+        <v>7</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>3</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>6</v>
+      </c>
+      <c r="F45" t="n">
+        <v>12</v>
+      </c>
+      <c r="G45" t="n">
+        <v>15</v>
+      </c>
+      <c r="H45" t="n">
+        <v>5</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>